<commit_message>
Added cluster all feature
</commit_message>
<xml_diff>
--- a/Tables/T0_vs_Energy.xlsx
+++ b/Tables/T0_vs_Energy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbackis/Documents/MultiGridAnalysisMesytec/Tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbackis/Documents/MultiGridAnalysis/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D952718D-1059-7B49-859C-AA0F915396C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A8BD22-BEB1-A14D-ACD5-CCC3303B82AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9920" yWindow="-6240" windowWidth="10000" windowHeight="23540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17600" yWindow="1080" windowWidth="14140" windowHeight="27720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="103">
   <si>
     <t>Van__3x3_High_Flux_Calibration_40.8</t>
   </si>
@@ -310,16 +310,47 @@
   </si>
   <si>
     <t>Van__3x3_High_Flux_Calibration_31.7</t>
+  </si>
+  <si>
+    <t>C4H2I2S_21.0</t>
+  </si>
+  <si>
+    <t>C4H2I2S_35.0</t>
+  </si>
+  <si>
+    <t>C4H2I2S_50.0</t>
+  </si>
+  <si>
+    <t>C4H2I2S_70.0</t>
+  </si>
+  <si>
+    <t>C4H2I2S_100.0</t>
+  </si>
+  <si>
+    <t>C4H2I2S_200.0</t>
+  </si>
+  <si>
+    <t>C4H2I2S_300.0</t>
+  </si>
+  <si>
+    <t>C4H2I2S_500.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -351,12 +382,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C96"/>
+  <dimension ref="A1:C104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1489,6 +1521,70 @@
         <v>52.455368551699998</v>
       </c>
     </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>95</v>
+      </c>
+      <c r="B97" s="1">
+        <v>41.479470892400002</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>96</v>
+      </c>
+      <c r="B98" s="1">
+        <v>49.964147709700001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>97</v>
+      </c>
+      <c r="B99" s="1">
+        <v>46.979429947900002</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>98</v>
+      </c>
+      <c r="B100" s="1">
+        <v>44.888850494899998</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B101" s="1">
+        <v>35.434604822099999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B102" s="1">
+        <v>14.3439196436</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B103" s="1">
+        <v>10.000636589100001</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B104" s="1">
+        <v>7.5932220974</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>